<commit_message>
Created discretization for heart_failure dataset.
</commit_message>
<xml_diff>
--- a/ProjectProgress.xlsx
+++ b/ProjectProgress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ac5a4a0f1d39cd7/Ambiente de Trabalho/cdados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1210" documentId="8_{A974636F-80FB-48E8-A277-64DF1B0FC152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C4F8E1F0-A63A-4C7E-A9E7-E29FEB710CAE}"/>
+  <xr:revisionPtr revIDLastSave="1225" documentId="8_{A974636F-80FB-48E8-A277-64DF1B0FC152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3367EB0C-5A97-4CF5-BF3D-E5E165269012}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{A9BC76B5-99E5-4818-92A9-7090B605E115}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="105">
   <si>
     <t>Data Profiling</t>
   </si>
@@ -277,9 +277,6 @@
     <t>F2 - 10 features (0, 1, 2, 3, 4, 5, 120, 214, 449, 997)</t>
   </si>
   <si>
-    <t>Naive Bayes - Feature Selection (reducing dataset to 10 features lead to the same results with less computational resources)</t>
-  </si>
-  <si>
     <t>KNN - Balancing did not improve results</t>
   </si>
   <si>
@@ -332,13 +329,34 @@
   </si>
   <si>
     <t>KNN had overall Better results than Multinomial NB</t>
+  </si>
+  <si>
+    <t>KNN: Manhattan with 13 neighbors had the best overall performance</t>
+  </si>
+  <si>
+    <t>Naive Bayes - feature selection had serious implications on recall results</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Negative</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Specificity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,6 +389,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -976,7 +1001,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1011,9 +1036,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1120,6 +1142,48 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1199,12 +1263,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1523,14 +1581,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{495C2598-04D0-473B-975C-E92B9F89DCF3}">
   <dimension ref="B3:BK26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A2" zoomScale="106" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.265625" customWidth="1"/>
+    <col min="6" max="6" width="14.265625" customWidth="1"/>
     <col min="7" max="7" width="13.73046875" customWidth="1"/>
     <col min="8" max="47" width="2.59765625" customWidth="1"/>
   </cols>
@@ -1541,164 +1599,164 @@
       </c>
     </row>
     <row r="4" spans="2:63" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="67"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="76" t="s">
+      <c r="B4" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="80"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="77"/>
-      <c r="M4" s="77"/>
-      <c r="N4" s="77"/>
-      <c r="O4" s="77"/>
-      <c r="P4" s="77"/>
-      <c r="Q4" s="77"/>
-      <c r="R4" s="77"/>
-      <c r="S4" s="77"/>
-      <c r="T4" s="77"/>
-      <c r="U4" s="77"/>
-      <c r="V4" s="77"/>
-      <c r="W4" s="77"/>
-      <c r="X4" s="77"/>
-      <c r="Y4" s="60" t="s">
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="90"/>
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="90"/>
+      <c r="W4" s="90"/>
+      <c r="X4" s="90"/>
+      <c r="Y4" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="Z4" s="61"/>
-      <c r="AA4" s="61"/>
-      <c r="AB4" s="61"/>
-      <c r="AC4" s="61"/>
-      <c r="AD4" s="62"/>
+      <c r="Z4" s="74"/>
+      <c r="AA4" s="74"/>
+      <c r="AB4" s="74"/>
+      <c r="AC4" s="74"/>
+      <c r="AD4" s="75"/>
     </row>
     <row r="5" spans="2:63" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="58" t="s">
+      <c r="F5" s="24"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="58" t="s">
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="59"/>
-      <c r="S5" s="59"/>
-      <c r="T5" s="58" t="s">
+      <c r="P5" s="72"/>
+      <c r="Q5" s="72"/>
+      <c r="R5" s="72"/>
+      <c r="S5" s="72"/>
+      <c r="T5" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="U5" s="59"/>
-      <c r="V5" s="59"/>
-      <c r="W5" s="59"/>
-      <c r="X5" s="59"/>
-      <c r="Y5" s="63"/>
-      <c r="Z5" s="64"/>
-      <c r="AA5" s="64"/>
-      <c r="AB5" s="64"/>
-      <c r="AC5" s="64"/>
-      <c r="AD5" s="65"/>
+      <c r="U5" s="72"/>
+      <c r="V5" s="72"/>
+      <c r="W5" s="72"/>
+      <c r="X5" s="72"/>
+      <c r="Y5" s="76"/>
+      <c r="Z5" s="77"/>
+      <c r="AA5" s="77"/>
+      <c r="AB5" s="77"/>
+      <c r="AC5" s="77"/>
+      <c r="AD5" s="78"/>
     </row>
     <row r="6" spans="2:63" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="F6" s="68" t="s">
+      <c r="F6" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="69"/>
-      <c r="H6" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="P6" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q6" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="R6" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="S6" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="T6" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="U6" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="V6" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="W6" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="X6" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y6" s="43" t="s">
+      <c r="G6" s="82"/>
+      <c r="H6" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="P6" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="T6" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="U6" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="V6" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="W6" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="X6" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y6" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="Z6" s="44" t="s">
+      <c r="Z6" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="AA6" s="44" t="s">
+      <c r="AA6" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="AB6" s="45" t="s">
+      <c r="AB6" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="AC6" s="45" t="s">
+      <c r="AC6" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="AD6" s="46" t="s">
+      <c r="AD6" s="45" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="7" spans="2:63" x14ac:dyDescent="0.45">
-      <c r="F7" s="74" t="s">
+      <c r="F7" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="32"/>
+      <c r="H7" s="31"/>
       <c r="I7" s="3" t="s">
         <v>19</v>
       </c>
@@ -1708,8 +1766,8 @@
         <v>38</v>
       </c>
       <c r="M7" s="3"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="32"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="31"/>
       <c r="P7" s="3" t="s">
         <v>19</v>
       </c>
@@ -1718,7 +1776,7 @@
       <c r="S7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="T7" s="32"/>
+      <c r="T7" s="31"/>
       <c r="U7" s="3" t="s">
         <v>19</v>
       </c>
@@ -1727,21 +1785,21 @@
       <c r="X7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="Y7" s="32"/>
+      <c r="Y7" s="31"/>
       <c r="Z7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AA7" s="20"/>
-      <c r="AB7" s="40"/>
-      <c r="AC7" s="40"/>
-      <c r="AD7" s="33"/>
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="39"/>
+      <c r="AC7" s="39"/>
+      <c r="AD7" s="32"/>
     </row>
     <row r="8" spans="2:63" x14ac:dyDescent="0.45">
-      <c r="F8" s="56"/>
-      <c r="G8" s="28" t="s">
+      <c r="F8" s="69"/>
+      <c r="G8" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="32"/>
+      <c r="H8" s="31"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3" t="s">
         <v>19</v>
@@ -1751,8 +1809,8 @@
         <v>0</v>
       </c>
       <c r="M8" s="3"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="32"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="31"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3" t="s">
         <v>19</v>
@@ -1761,7 +1819,7 @@
       <c r="S8" s="3">
         <v>0</v>
       </c>
-      <c r="T8" s="32"/>
+      <c r="T8" s="31"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3" t="s">
         <v>19</v>
@@ -1770,21 +1828,21 @@
       <c r="X8" s="3">
         <v>0</v>
       </c>
-      <c r="Y8" s="32"/>
+      <c r="Y8" s="31"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AB8" s="22"/>
-      <c r="AC8" s="22"/>
-      <c r="AD8" s="33"/>
+      <c r="AB8" s="21"/>
+      <c r="AC8" s="21"/>
+      <c r="AD8" s="32"/>
     </row>
     <row r="9" spans="2:63" x14ac:dyDescent="0.45">
-      <c r="F9" s="75"/>
-      <c r="G9" s="28" t="s">
+      <c r="F9" s="88"/>
+      <c r="G9" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="32"/>
+      <c r="H9" s="31"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3" t="s">
@@ -1792,38 +1850,38 @@
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="32"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="31"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="S9" s="3"/>
-      <c r="T9" s="32"/>
+      <c r="T9" s="31"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="X9" s="3"/>
-      <c r="Y9" s="32"/>
+      <c r="Y9" s="31"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
-      <c r="AB9" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC9" s="22"/>
-      <c r="AD9" s="33"/>
+      <c r="AB9" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC9" s="21"/>
+      <c r="AD9" s="32"/>
     </row>
     <row r="10" spans="2:63" x14ac:dyDescent="0.45">
-      <c r="F10" s="74" t="s">
+      <c r="F10" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="H10" s="34"/>
+      <c r="H10" s="33"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -1831,65 +1889,65 @@
       <c r="M10" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="N10" s="24" t="s">
+      <c r="N10" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="O10" s="34"/>
+      <c r="O10" s="33"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
-      <c r="T10" s="34"/>
+      <c r="T10" s="33"/>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
-      <c r="Y10" s="32"/>
+      <c r="Y10" s="31"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
-      <c r="AB10" s="22"/>
-      <c r="AC10" s="22" t="s">
+      <c r="AB10" s="21"/>
+      <c r="AC10" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD10" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="AD10" s="33" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="11" spans="2:63" x14ac:dyDescent="0.45">
-      <c r="F11" s="75"/>
-      <c r="G11" s="29" t="s">
+      <c r="F11" s="88"/>
+      <c r="G11" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="34"/>
+      <c r="H11" s="33"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="34"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="33"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
-      <c r="T11" s="34"/>
+      <c r="T11" s="33"/>
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
-      <c r="Y11" s="32"/>
+      <c r="Y11" s="31"/>
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
-      <c r="AB11" s="22"/>
-      <c r="AC11" s="22"/>
-      <c r="AD11" s="33"/>
+      <c r="AB11" s="21"/>
+      <c r="AC11" s="21"/>
+      <c r="AD11" s="32"/>
     </row>
     <row r="12" spans="2:63" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="F12" s="70" t="s">
+      <c r="F12" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="71"/>
-      <c r="H12" s="34" t="s">
+      <c r="G12" s="84"/>
+      <c r="H12" s="33" t="s">
         <v>21</v>
       </c>
       <c r="I12" s="4" t="s">
@@ -1907,10 +1965,10 @@
       <c r="M12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="N12" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="O12" s="34" t="s">
+      <c r="N12" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12" s="33" t="s">
         <v>21</v>
       </c>
       <c r="P12" s="4" t="s">
@@ -1925,7 +1983,7 @@
       <c r="S12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="T12" s="34" t="s">
+      <c r="T12" s="33" t="s">
         <v>21</v>
       </c>
       <c r="U12" s="4" t="s">
@@ -1940,7 +1998,7 @@
       <c r="X12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Y12" s="38" t="s">
+      <c r="Y12" s="37" t="s">
         <v>21</v>
       </c>
       <c r="Z12" s="5" t="s">
@@ -1949,257 +2007,257 @@
       <c r="AA12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AB12" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC12" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="AD12" s="39" t="s">
+      <c r="AB12" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC12" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD12" s="38" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:63" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="F13" s="55" t="s">
+      <c r="F13" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="36">
+      <c r="H13" s="56">
         <v>85</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="57">
         <v>77</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="57">
         <v>80</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="57">
         <v>86</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="57">
         <v>85</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="57">
         <v>92</v>
       </c>
-      <c r="N13" s="21">
+      <c r="N13" s="58">
         <v>92</v>
       </c>
-      <c r="O13" s="36">
+      <c r="O13" s="56">
         <v>76</v>
       </c>
-      <c r="P13" s="6">
+      <c r="P13" s="57">
         <v>72</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="Q13" s="57">
         <v>75</v>
       </c>
-      <c r="R13" s="6">
+      <c r="R13" s="57">
         <v>81</v>
       </c>
-      <c r="S13" s="6">
+      <c r="S13" s="57">
         <v>77</v>
       </c>
-      <c r="T13" s="36">
+      <c r="T13" s="56">
         <v>79</v>
       </c>
-      <c r="U13" s="6">
+      <c r="U13" s="57">
         <v>71</v>
       </c>
-      <c r="V13" s="6">
+      <c r="V13" s="57">
         <v>72</v>
       </c>
-      <c r="W13" s="6">
+      <c r="W13" s="57">
         <v>71</v>
       </c>
-      <c r="X13" s="6">
+      <c r="X13" s="57">
         <v>79</v>
       </c>
-      <c r="Y13" s="36">
+      <c r="Y13" s="56">
         <v>93</v>
       </c>
-      <c r="Z13" s="6">
+      <c r="Z13" s="57">
         <v>85</v>
       </c>
-      <c r="AA13" s="6">
+      <c r="AA13" s="57">
         <v>92</v>
       </c>
-      <c r="AB13" s="21">
+      <c r="AB13" s="58">
         <v>89</v>
       </c>
-      <c r="AC13" s="21">
+      <c r="AC13" s="58">
         <v>92</v>
       </c>
-      <c r="AD13" s="37">
+      <c r="AD13" s="59">
         <v>91</v>
       </c>
     </row>
     <row r="14" spans="2:63" x14ac:dyDescent="0.45">
-      <c r="F14" s="56"/>
-      <c r="G14" s="28" t="s">
+      <c r="F14" s="69"/>
+      <c r="G14" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="32">
+      <c r="H14" s="60">
         <v>61</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="61">
         <v>70</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="61">
         <v>69</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="61">
         <v>56</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14" s="61">
         <v>61</v>
       </c>
-      <c r="M14" s="3">
+      <c r="M14" s="61">
         <v>11</v>
       </c>
-      <c r="N14" s="22">
+      <c r="N14" s="62">
         <v>11</v>
       </c>
-      <c r="O14" s="32">
+      <c r="O14" s="60">
         <v>70</v>
       </c>
-      <c r="P14" s="3">
+      <c r="P14" s="61">
         <v>73</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="Q14" s="61">
         <v>70</v>
       </c>
-      <c r="R14" s="3">
+      <c r="R14" s="61">
         <v>34</v>
       </c>
-      <c r="S14" s="3">
+      <c r="S14" s="61">
         <v>71</v>
       </c>
-      <c r="T14" s="32">
+      <c r="T14" s="60">
         <v>66</v>
       </c>
-      <c r="U14" s="3">
+      <c r="U14" s="61">
         <v>72</v>
       </c>
-      <c r="V14" s="3">
+      <c r="V14" s="61">
         <v>71</v>
       </c>
-      <c r="W14" s="3">
+      <c r="W14" s="61">
         <v>61</v>
       </c>
-      <c r="X14" s="3">
+      <c r="X14" s="61">
         <v>66</v>
       </c>
-      <c r="Y14" s="32">
+      <c r="Y14" s="60">
         <v>53</v>
       </c>
-      <c r="Z14" s="3">
+      <c r="Z14" s="61">
         <v>33</v>
       </c>
-      <c r="AA14" s="3">
+      <c r="AA14" s="61">
         <v>53</v>
       </c>
-      <c r="AB14" s="22">
+      <c r="AB14" s="62">
         <v>4</v>
       </c>
-      <c r="AC14" s="22">
+      <c r="AC14" s="62">
         <v>22</v>
       </c>
-      <c r="AD14" s="33">
+      <c r="AD14" s="63">
         <v>24</v>
       </c>
-      <c r="AU14" s="19"/>
-      <c r="AV14" s="19"/>
-      <c r="AW14" s="19"/>
-      <c r="AX14" s="19"/>
-      <c r="AY14" s="19"/>
-      <c r="AZ14" s="19"/>
-      <c r="BA14" s="19"/>
-      <c r="BB14" s="19"/>
-      <c r="BC14" s="19"/>
-      <c r="BD14" s="19"/>
-      <c r="BE14" s="19"/>
-      <c r="BF14" s="19"/>
-      <c r="BG14" s="19"/>
-      <c r="BH14" s="19"/>
-      <c r="BI14" s="19"/>
-      <c r="BJ14" s="19"/>
-      <c r="BK14" s="19"/>
+      <c r="AU14" s="18"/>
+      <c r="AV14" s="18"/>
+      <c r="AW14" s="18"/>
+      <c r="AX14" s="18"/>
+      <c r="AY14" s="18"/>
+      <c r="AZ14" s="18"/>
+      <c r="BA14" s="18"/>
+      <c r="BB14" s="18"/>
+      <c r="BC14" s="18"/>
+      <c r="BD14" s="18"/>
+      <c r="BE14" s="18"/>
+      <c r="BF14" s="18"/>
+      <c r="BG14" s="18"/>
+      <c r="BH14" s="18"/>
+      <c r="BI14" s="18"/>
+      <c r="BJ14" s="18"/>
+      <c r="BK14" s="18"/>
     </row>
     <row r="15" spans="2:63" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="F15" s="57"/>
-      <c r="G15" s="31" t="s">
+      <c r="F15" s="70"/>
+      <c r="G15" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="38">
+      <c r="H15" s="64">
         <v>31</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="65">
         <v>22</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="65">
         <v>24</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K15" s="65">
         <v>31</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="65">
         <v>31</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15" s="65">
         <v>79</v>
       </c>
-      <c r="N15" s="23">
+      <c r="N15" s="66">
         <v>81</v>
       </c>
-      <c r="O15" s="38">
-        <v>21</v>
-      </c>
-      <c r="P15" s="5">
-        <v>19</v>
-      </c>
-      <c r="Q15" s="5">
+      <c r="O15" s="64">
+        <v>21</v>
+      </c>
+      <c r="P15" s="65">
+        <v>19</v>
+      </c>
+      <c r="Q15" s="65">
         <v>20</v>
       </c>
-      <c r="R15" s="5">
+      <c r="R15" s="65">
         <v>17</v>
       </c>
-      <c r="S15" s="5">
+      <c r="S15" s="65">
         <v>22</v>
       </c>
-      <c r="T15" s="38">
+      <c r="T15" s="64">
         <v>23</v>
       </c>
-      <c r="U15" s="5">
+      <c r="U15" s="65">
         <v>18</v>
       </c>
-      <c r="V15" s="5">
-        <v>19</v>
-      </c>
-      <c r="W15" s="5">
+      <c r="V15" s="65">
+        <v>19</v>
+      </c>
+      <c r="W15" s="65">
         <v>16</v>
       </c>
-      <c r="X15" s="5">
+      <c r="X15" s="65">
         <v>23</v>
       </c>
-      <c r="Y15" s="38">
+      <c r="Y15" s="64">
         <v>61</v>
       </c>
-      <c r="Z15" s="5">
+      <c r="Z15" s="65">
         <v>22</v>
       </c>
-      <c r="AA15" s="5">
+      <c r="AA15" s="65">
         <v>54</v>
       </c>
-      <c r="AB15" s="23">
+      <c r="AB15" s="66">
         <v>12</v>
       </c>
-      <c r="AC15" s="23">
+      <c r="AC15" s="66">
         <v>62</v>
       </c>
-      <c r="AD15" s="39">
+      <c r="AD15" s="67">
         <v>41</v>
       </c>
     </row>
@@ -2219,7 +2277,7 @@
         <v>26</v>
       </c>
       <c r="H19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.45">
@@ -2227,7 +2285,7 @@
         <v>27</v>
       </c>
       <c r="H20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.45">
@@ -2237,28 +2295,28 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2319,313 +2377,313 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319FC6BD-9C11-44F3-8E55-49648E999F9A}">
-  <dimension ref="B3:BC35"/>
+  <dimension ref="B3:BG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R2" zoomScale="105" zoomScaleNormal="328" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="105" zoomScaleNormal="328" workbookViewId="0">
+      <selection activeCell="BF13" sqref="BF13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.265625" customWidth="1"/>
+    <col min="6" max="6" width="14.265625" customWidth="1"/>
     <col min="7" max="7" width="13.73046875" customWidth="1"/>
-    <col min="8" max="55" width="2.796875" customWidth="1"/>
+    <col min="8" max="55" width="2.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:55" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:59" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="F3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:55" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="67"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="76" t="s">
+    <row r="4" spans="2:59" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B4" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="80"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="77"/>
-      <c r="M4" s="77"/>
-      <c r="N4" s="77"/>
-      <c r="O4" s="77"/>
-      <c r="P4" s="77"/>
-      <c r="Q4" s="77"/>
-      <c r="R4" s="77"/>
-      <c r="S4" s="77"/>
-      <c r="T4" s="77"/>
-      <c r="U4" s="77"/>
-      <c r="V4" s="77"/>
-      <c r="W4" s="77"/>
-      <c r="X4" s="77"/>
-      <c r="Y4" s="77"/>
-      <c r="Z4" s="77"/>
-      <c r="AA4" s="77"/>
-      <c r="AB4" s="77"/>
-      <c r="AC4" s="77"/>
-      <c r="AD4" s="77"/>
-      <c r="AE4" s="77"/>
-      <c r="AF4" s="77"/>
-      <c r="AG4" s="77"/>
-      <c r="AH4" s="77"/>
-      <c r="AI4" s="77"/>
-      <c r="AJ4" s="77"/>
-      <c r="AK4" s="77"/>
-      <c r="AL4" s="77"/>
-      <c r="AM4" s="77"/>
-      <c r="AN4" s="77"/>
-      <c r="AO4" s="77"/>
-      <c r="AP4" s="77"/>
-      <c r="AQ4" s="77"/>
-      <c r="AR4" s="77"/>
-      <c r="AS4" s="78"/>
-      <c r="AT4" s="63" t="s">
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="90"/>
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="90"/>
+      <c r="W4" s="90"/>
+      <c r="X4" s="90"/>
+      <c r="Y4" s="90"/>
+      <c r="Z4" s="90"/>
+      <c r="AA4" s="90"/>
+      <c r="AB4" s="90"/>
+      <c r="AC4" s="90"/>
+      <c r="AD4" s="90"/>
+      <c r="AE4" s="90"/>
+      <c r="AF4" s="90"/>
+      <c r="AG4" s="90"/>
+      <c r="AH4" s="90"/>
+      <c r="AI4" s="90"/>
+      <c r="AJ4" s="90"/>
+      <c r="AK4" s="90"/>
+      <c r="AL4" s="90"/>
+      <c r="AM4" s="90"/>
+      <c r="AN4" s="90"/>
+      <c r="AO4" s="90"/>
+      <c r="AP4" s="90"/>
+      <c r="AQ4" s="90"/>
+      <c r="AR4" s="90"/>
+      <c r="AS4" s="91"/>
+      <c r="AT4" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="AU4" s="64"/>
-      <c r="AV4" s="64"/>
-      <c r="AW4" s="64"/>
-      <c r="AX4" s="64"/>
-      <c r="AY4" s="64"/>
-      <c r="AZ4" s="64"/>
-      <c r="BA4" s="64"/>
-      <c r="BB4" s="64"/>
-      <c r="BC4" s="64"/>
-    </row>
-    <row r="5" spans="2:55" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="AU4" s="77"/>
+      <c r="AV4" s="77"/>
+      <c r="AW4" s="77"/>
+      <c r="AX4" s="77"/>
+      <c r="AY4" s="77"/>
+      <c r="AZ4" s="77"/>
+      <c r="BA4" s="77"/>
+      <c r="BB4" s="77"/>
+      <c r="BC4" s="77"/>
+    </row>
+    <row r="5" spans="2:59" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="72" t="s">
+      <c r="F5" s="24"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="79"/>
-      <c r="N5" s="79"/>
-      <c r="O5" s="79"/>
-      <c r="P5" s="79"/>
-      <c r="Q5" s="79"/>
-      <c r="R5" s="79"/>
-      <c r="S5" s="73"/>
-      <c r="T5" s="72" t="s">
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="92"/>
+      <c r="N5" s="92"/>
+      <c r="O5" s="92"/>
+      <c r="P5" s="92"/>
+      <c r="Q5" s="92"/>
+      <c r="R5" s="92"/>
+      <c r="S5" s="86"/>
+      <c r="T5" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="U5" s="79"/>
-      <c r="V5" s="79"/>
-      <c r="W5" s="79"/>
-      <c r="X5" s="79"/>
-      <c r="Y5" s="79"/>
-      <c r="Z5" s="79"/>
-      <c r="AA5" s="79"/>
-      <c r="AB5" s="79"/>
-      <c r="AC5" s="79"/>
-      <c r="AD5" s="79"/>
-      <c r="AE5" s="79"/>
-      <c r="AF5" s="79"/>
-      <c r="AG5" s="79"/>
-      <c r="AH5" s="79"/>
-      <c r="AI5" s="73"/>
-      <c r="AJ5" s="72" t="s">
+      <c r="U5" s="92"/>
+      <c r="V5" s="92"/>
+      <c r="W5" s="92"/>
+      <c r="X5" s="92"/>
+      <c r="Y5" s="92"/>
+      <c r="Z5" s="92"/>
+      <c r="AA5" s="92"/>
+      <c r="AB5" s="92"/>
+      <c r="AC5" s="92"/>
+      <c r="AD5" s="92"/>
+      <c r="AE5" s="92"/>
+      <c r="AF5" s="92"/>
+      <c r="AG5" s="92"/>
+      <c r="AH5" s="92"/>
+      <c r="AI5" s="86"/>
+      <c r="AJ5" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="AK5" s="79"/>
-      <c r="AL5" s="79"/>
-      <c r="AM5" s="79"/>
-      <c r="AN5" s="79"/>
-      <c r="AO5" s="79"/>
-      <c r="AP5" s="79"/>
-      <c r="AQ5" s="79"/>
-      <c r="AR5" s="79"/>
-      <c r="AS5" s="73"/>
-      <c r="AT5" s="63"/>
-      <c r="AU5" s="64"/>
-      <c r="AV5" s="64"/>
-      <c r="AW5" s="64"/>
-      <c r="AX5" s="64"/>
-      <c r="AY5" s="64"/>
-      <c r="AZ5" s="64"/>
-      <c r="BA5" s="64"/>
-      <c r="BB5" s="64"/>
-      <c r="BC5" s="64"/>
-    </row>
-    <row r="6" spans="2:55" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="AK5" s="92"/>
+      <c r="AL5" s="92"/>
+      <c r="AM5" s="92"/>
+      <c r="AN5" s="92"/>
+      <c r="AO5" s="92"/>
+      <c r="AP5" s="92"/>
+      <c r="AQ5" s="92"/>
+      <c r="AR5" s="92"/>
+      <c r="AS5" s="86"/>
+      <c r="AT5" s="76"/>
+      <c r="AU5" s="77"/>
+      <c r="AV5" s="77"/>
+      <c r="AW5" s="77"/>
+      <c r="AX5" s="77"/>
+      <c r="AY5" s="77"/>
+      <c r="AZ5" s="77"/>
+      <c r="BA5" s="77"/>
+      <c r="BB5" s="77"/>
+      <c r="BC5" s="77"/>
+    </row>
+    <row r="6" spans="2:59" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="F6" s="68" t="s">
+      <c r="F6" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="69"/>
-      <c r="H6" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="P6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="R6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="S6" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="T6" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="U6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="V6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="W6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="X6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AH6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AI6" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="AJ6" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="AK6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AM6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AN6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AO6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AP6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AQ6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AR6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="AS6" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="AT6" s="52" t="s">
+      <c r="G6" s="82"/>
+      <c r="H6" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="P6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="T6" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="U6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="V6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="W6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="X6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI6" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ6" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR6" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS6" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT6" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="AU6" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="AU6" s="53" t="s">
+      <c r="AV6" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="AW6" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="AV6" s="53" t="s">
-        <v>72</v>
-      </c>
-      <c r="AW6" s="82" t="s">
+      <c r="AX6" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="AX6" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="AY6" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="AZ6" s="83" t="s">
-        <v>87</v>
-      </c>
-      <c r="BA6" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="BB6" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="BC6" s="54" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="2:55" x14ac:dyDescent="0.45">
+      <c r="AY6" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="AZ6" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="BA6" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="BB6" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="BC6" s="53" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="2:59" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="F7" s="74" t="s">
+      <c r="F7" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="32"/>
+      <c r="H7" s="31"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -2636,8 +2694,8 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
-      <c r="S7" s="33"/>
-      <c r="T7" s="32"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="31"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
@@ -2660,8 +2718,8 @@
       <c r="AH7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AI7" s="33"/>
-      <c r="AJ7" s="32"/>
+      <c r="AI7" s="32"/>
+      <c r="AJ7" s="31"/>
       <c r="AK7" s="3"/>
       <c r="AL7" s="3"/>
       <c r="AM7" s="3"/>
@@ -2672,34 +2730,40 @@
       <c r="AP7" s="8"/>
       <c r="AQ7" s="3"/>
       <c r="AR7" s="3"/>
-      <c r="AS7" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="AT7" s="32"/>
+      <c r="AS7" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT7" s="31"/>
       <c r="AU7" s="3"/>
-      <c r="AV7" s="20"/>
-      <c r="AW7" s="22"/>
+      <c r="AV7" s="19"/>
+      <c r="AW7" s="21"/>
       <c r="AX7" s="3"/>
       <c r="AY7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AZ7" s="8"/>
-      <c r="BA7" s="20"/>
+      <c r="BA7" s="19"/>
       <c r="BB7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="BC7" s="33"/>
-    </row>
-    <row r="8" spans="2:55" x14ac:dyDescent="0.45">
+      <c r="BC7" s="32"/>
+      <c r="BF7" t="s">
+        <v>100</v>
+      </c>
+      <c r="BG7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="2:59" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="28" t="s">
+      <c r="F8" s="88"/>
+      <c r="G8" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="32"/>
+      <c r="H8" s="31"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -2716,10 +2780,10 @@
         <v>19</v>
       </c>
       <c r="R8" s="3"/>
-      <c r="S8" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="T8" s="32"/>
+      <c r="S8" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="T8" s="31"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
@@ -2740,10 +2804,10 @@
       </c>
       <c r="AG8" s="3"/>
       <c r="AH8" s="3"/>
-      <c r="AI8" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="AJ8" s="32"/>
+      <c r="AI8" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ8" s="31"/>
       <c r="AK8" s="3"/>
       <c r="AL8" s="3"/>
       <c r="AM8" s="3"/>
@@ -2756,28 +2820,31 @@
       <c r="AR8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AS8" s="22"/>
-      <c r="AT8" s="32"/>
+      <c r="AS8" s="21"/>
+      <c r="AT8" s="31"/>
       <c r="AU8" s="3"/>
-      <c r="AV8" s="20"/>
-      <c r="AW8" s="22"/>
+      <c r="AV8" s="19"/>
+      <c r="AW8" s="21"/>
       <c r="AX8" s="3"/>
       <c r="AY8" s="3"/>
       <c r="AZ8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="BA8" s="20"/>
+      <c r="BA8" s="19"/>
       <c r="BB8" s="3"/>
-      <c r="BC8" s="33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="2:55" x14ac:dyDescent="0.45">
-      <c r="F9" s="80" t="s">
+      <c r="BC8" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="BE8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="2:59" x14ac:dyDescent="0.45">
+      <c r="F9" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="81"/>
-      <c r="H9" s="32"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="31"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -2798,10 +2865,10 @@
       <c r="R9" s="3">
         <v>0</v>
       </c>
-      <c r="S9" s="33">
-        <v>0</v>
-      </c>
-      <c r="T9" s="32"/>
+      <c r="S9" s="32">
+        <v>0</v>
+      </c>
+      <c r="T9" s="31"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
@@ -2832,8 +2899,8 @@
       <c r="AH9" s="3">
         <v>0</v>
       </c>
-      <c r="AI9" s="33"/>
-      <c r="AJ9" s="32"/>
+      <c r="AI9" s="32"/>
+      <c r="AJ9" s="31"/>
       <c r="AK9" s="3"/>
       <c r="AL9" s="3"/>
       <c r="AM9" s="3"/>
@@ -2846,34 +2913,37 @@
       <c r="AR9" s="3">
         <v>1</v>
       </c>
-      <c r="AS9" s="22">
-        <v>0</v>
-      </c>
-      <c r="AT9" s="32"/>
+      <c r="AS9" s="21">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="31"/>
       <c r="AU9" s="3"/>
-      <c r="AV9" s="20"/>
-      <c r="AW9" s="22"/>
+      <c r="AV9" s="19"/>
+      <c r="AW9" s="21"/>
       <c r="AX9" s="3"/>
       <c r="AY9" s="3"/>
       <c r="AZ9" s="8"/>
-      <c r="BA9" s="20">
+      <c r="BA9" s="19">
         <v>0</v>
       </c>
       <c r="BB9" s="3">
         <v>0</v>
       </c>
-      <c r="BC9" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:55" x14ac:dyDescent="0.45">
-      <c r="F10" s="74" t="s">
+      <c r="BC9" s="32">
+        <v>0</v>
+      </c>
+      <c r="BE9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="2:59" x14ac:dyDescent="0.45">
+      <c r="F10" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="32"/>
+      <c r="H10" s="31"/>
       <c r="I10" s="3" t="s">
         <v>19</v>
       </c>
@@ -2900,10 +2970,10 @@
       <c r="R10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="S10" s="33" t="s">
+      <c r="S10" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="T10" s="32"/>
+      <c r="T10" s="31"/>
       <c r="U10" s="3" t="s">
         <v>19</v>
       </c>
@@ -2942,8 +3012,8 @@
       <c r="AH10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AI10" s="33"/>
-      <c r="AJ10" s="32"/>
+      <c r="AI10" s="32"/>
+      <c r="AJ10" s="31"/>
       <c r="AK10" s="3" t="s">
         <v>19</v>
       </c>
@@ -2964,15 +3034,15 @@
       <c r="AR10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AS10" s="22" t="s">
+      <c r="AS10" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="AT10" s="32"/>
+      <c r="AT10" s="31"/>
       <c r="AU10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AV10" s="20"/>
-      <c r="AW10" s="22"/>
+      <c r="AV10" s="19"/>
+      <c r="AW10" s="21"/>
       <c r="AX10" s="3" t="s">
         <v>34</v>
       </c>
@@ -2982,22 +3052,22 @@
       <c r="AZ10" s="8">
         <v>0</v>
       </c>
-      <c r="BA10" s="20">
+      <c r="BA10" s="19">
         <v>0</v>
       </c>
       <c r="BB10" s="3">
         <v>0</v>
       </c>
-      <c r="BC10" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:55" x14ac:dyDescent="0.45">
-      <c r="F11" s="56"/>
-      <c r="G11" s="28" t="s">
+      <c r="BC10" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:59" x14ac:dyDescent="0.45">
+      <c r="F11" s="69"/>
+      <c r="G11" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="32"/>
+      <c r="H11" s="31"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3" t="s">
         <v>19</v>
@@ -3024,10 +3094,10 @@
       <c r="R11" s="3">
         <v>0</v>
       </c>
-      <c r="S11" s="33" t="s">
+      <c r="S11" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="T11" s="32"/>
+      <c r="T11" s="31"/>
       <c r="U11" s="3"/>
       <c r="V11" s="3" t="s">
         <v>19</v>
@@ -3066,8 +3136,8 @@
       <c r="AH11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AI11" s="33"/>
-      <c r="AJ11" s="32"/>
+      <c r="AI11" s="32"/>
+      <c r="AJ11" s="31"/>
       <c r="AK11" s="3"/>
       <c r="AL11" s="3" t="s">
         <v>19</v>
@@ -3088,15 +3158,15 @@
       <c r="AR11" s="3">
         <v>0</v>
       </c>
-      <c r="AS11" s="22">
-        <v>0</v>
-      </c>
-      <c r="AT11" s="32"/>
+      <c r="AS11" s="21">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="31"/>
       <c r="AU11" s="3"/>
       <c r="AV11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AW11" s="22"/>
+      <c r="AW11" s="21"/>
       <c r="AX11" s="3" t="s">
         <v>40</v>
       </c>
@@ -3112,16 +3182,23 @@
       <c r="BB11" s="3">
         <v>0</v>
       </c>
-      <c r="BC11" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:55" x14ac:dyDescent="0.45">
-      <c r="F12" s="75"/>
-      <c r="G12" s="28" t="s">
+      <c r="BC11" s="32">
+        <v>0</v>
+      </c>
+      <c r="BE11" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF11" t="e">
+        <f>(BF8+BG9)/(BF8+BG8+BF9+BG9)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="2:59" x14ac:dyDescent="0.45">
+      <c r="F12" s="88"/>
+      <c r="G12" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="32"/>
+      <c r="H12" s="31"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3" t="s">
@@ -3134,8 +3211,8 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
-      <c r="S12" s="33"/>
-      <c r="T12" s="32"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="31"/>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3" t="s">
@@ -3152,8 +3229,8 @@
       <c r="AF12" s="3"/>
       <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
-      <c r="AI12" s="33"/>
-      <c r="AJ12" s="32"/>
+      <c r="AI12" s="32"/>
+      <c r="AJ12" s="31"/>
       <c r="AK12" s="3"/>
       <c r="AL12" s="3"/>
       <c r="AM12" s="3" t="s">
@@ -3164,11 +3241,11 @@
       <c r="AP12" s="8"/>
       <c r="AQ12" s="3"/>
       <c r="AR12" s="3"/>
-      <c r="AS12" s="22"/>
-      <c r="AT12" s="32"/>
+      <c r="AS12" s="21"/>
+      <c r="AT12" s="31"/>
       <c r="AU12" s="3"/>
       <c r="AV12" s="3"/>
-      <c r="AW12" s="22" t="s">
+      <c r="AW12" s="21" t="s">
         <v>19</v>
       </c>
       <c r="AX12" s="3"/>
@@ -3176,16 +3253,19 @@
       <c r="AZ12" s="8"/>
       <c r="BA12" s="3"/>
       <c r="BB12" s="3"/>
-      <c r="BC12" s="33"/>
-    </row>
-    <row r="13" spans="2:55" x14ac:dyDescent="0.45">
-      <c r="F13" s="74" t="s">
+      <c r="BC12" s="32"/>
+      <c r="BE12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:59" x14ac:dyDescent="0.45">
+      <c r="F13" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="34"/>
+      <c r="H13" s="33"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -3200,8 +3280,8 @@
         <v>48</v>
       </c>
       <c r="R13" s="4"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="34"/>
+      <c r="S13" s="34"/>
+      <c r="T13" s="33"/>
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
@@ -3222,8 +3302,8 @@
       </c>
       <c r="AG13" s="4"/>
       <c r="AH13" s="4"/>
-      <c r="AI13" s="35"/>
-      <c r="AJ13" s="34"/>
+      <c r="AI13" s="34"/>
+      <c r="AJ13" s="33"/>
       <c r="AK13" s="4"/>
       <c r="AL13" s="4"/>
       <c r="AM13" s="4"/>
@@ -3232,24 +3312,27 @@
       <c r="AP13" s="9"/>
       <c r="AQ13" s="4"/>
       <c r="AR13" s="4"/>
-      <c r="AS13" s="24"/>
-      <c r="AT13" s="32"/>
+      <c r="AS13" s="23"/>
+      <c r="AT13" s="31"/>
       <c r="AU13" s="3"/>
       <c r="AV13" s="3"/>
-      <c r="AW13" s="22"/>
+      <c r="AW13" s="21"/>
       <c r="AX13" s="3"/>
       <c r="AY13" s="3"/>
       <c r="AZ13" s="8"/>
       <c r="BA13" s="3"/>
       <c r="BB13" s="3"/>
-      <c r="BC13" s="33"/>
-    </row>
-    <row r="14" spans="2:55" x14ac:dyDescent="0.45">
-      <c r="F14" s="75"/>
-      <c r="G14" s="29" t="s">
+      <c r="BC13" s="32"/>
+      <c r="BE13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="2:59" x14ac:dyDescent="0.45">
+      <c r="F14" s="88"/>
+      <c r="G14" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="H14" s="34"/>
+      <c r="H14" s="33"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -3262,10 +3345,10 @@
       <c r="R14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="S14" s="35" t="s">
+      <c r="S14" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="T14" s="34"/>
+      <c r="T14" s="33"/>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
@@ -3284,10 +3367,10 @@
       <c r="AH14" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AI14" s="35" t="s">
+      <c r="AI14" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="AJ14" s="34"/>
+      <c r="AJ14" s="33"/>
       <c r="AK14" s="4"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
@@ -3296,24 +3379,24 @@
       <c r="AP14" s="9"/>
       <c r="AQ14" s="4"/>
       <c r="AR14" s="4"/>
-      <c r="AS14" s="24"/>
-      <c r="AT14" s="32"/>
+      <c r="AS14" s="23"/>
+      <c r="AT14" s="31"/>
       <c r="AU14" s="3"/>
       <c r="AV14" s="3"/>
-      <c r="AW14" s="22"/>
+      <c r="AW14" s="21"/>
       <c r="AX14" s="3"/>
       <c r="AY14" s="3"/>
       <c r="AZ14" s="8"/>
       <c r="BA14" s="3"/>
       <c r="BB14" s="3"/>
-      <c r="BC14" s="33"/>
-    </row>
-    <row r="15" spans="2:55" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="F15" s="70" t="s">
+      <c r="BC14" s="32"/>
+    </row>
+    <row r="15" spans="2:59" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="F15" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="71"/>
-      <c r="H15" s="34" t="s">
+      <c r="G15" s="84"/>
+      <c r="H15" s="33" t="s">
         <v>21</v>
       </c>
       <c r="I15" s="4" t="s">
@@ -3346,10 +3429,10 @@
       <c r="R15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="S15" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="T15" s="34" t="s">
+      <c r="S15" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="T15" s="33" t="s">
         <v>21</v>
       </c>
       <c r="U15" s="4" t="s">
@@ -3394,10 +3477,10 @@
       <c r="AH15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AI15" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="AJ15" s="34" t="s">
+      <c r="AI15" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ15" s="33" t="s">
         <v>21</v>
       </c>
       <c r="AK15" s="4" t="s">
@@ -3424,28 +3507,28 @@
       <c r="AR15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AS15" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="AT15" s="34"/>
+      <c r="AS15" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="AT15" s="33"/>
       <c r="AU15" s="4"/>
       <c r="AV15" s="4"/>
-      <c r="AW15" s="24"/>
+      <c r="AW15" s="23"/>
       <c r="AX15" s="4"/>
       <c r="AY15" s="4"/>
       <c r="AZ15" s="9"/>
       <c r="BA15" s="4"/>
       <c r="BB15" s="4"/>
-      <c r="BC15" s="35"/>
-    </row>
-    <row r="16" spans="2:55" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="F16" s="55" t="s">
+      <c r="BC15" s="34"/>
+    </row>
+    <row r="16" spans="2:59" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="F16" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="36">
+      <c r="H16" s="35">
         <v>66</v>
       </c>
       <c r="I16" s="6">
@@ -3478,10 +3561,10 @@
       <c r="R16" s="6">
         <v>74</v>
       </c>
-      <c r="S16" s="37">
+      <c r="S16" s="36">
         <v>78</v>
       </c>
-      <c r="T16" s="36">
+      <c r="T16" s="35">
         <v>80</v>
       </c>
       <c r="U16" s="6">
@@ -3526,10 +3609,10 @@
       <c r="AH16" s="6">
         <v>84</v>
       </c>
-      <c r="AI16" s="37">
+      <c r="AI16" s="36">
         <v>84</v>
       </c>
-      <c r="AJ16" s="36">
+      <c r="AJ16" s="35">
         <v>68</v>
       </c>
       <c r="AK16" s="6">
@@ -3556,10 +3639,10 @@
       <c r="AR16" s="6">
         <v>75</v>
       </c>
-      <c r="AS16" s="21">
+      <c r="AS16" s="20">
         <v>71</v>
       </c>
-      <c r="AT16" s="36">
+      <c r="AT16" s="35">
         <v>65</v>
       </c>
       <c r="AU16" s="6">
@@ -3568,7 +3651,7 @@
       <c r="AV16" s="6">
         <v>51</v>
       </c>
-      <c r="AW16" s="21">
+      <c r="AW16" s="20">
         <v>51</v>
       </c>
       <c r="AX16" s="6">
@@ -3586,16 +3669,16 @@
       <c r="BB16" s="6">
         <v>76</v>
       </c>
-      <c r="BC16" s="37">
+      <c r="BC16" s="36">
         <v>75</v>
       </c>
     </row>
     <row r="17" spans="2:55" x14ac:dyDescent="0.45">
-      <c r="F17" s="56"/>
-      <c r="G17" s="28" t="s">
+      <c r="F17" s="69"/>
+      <c r="G17" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="31">
         <v>78</v>
       </c>
       <c r="I17" s="3">
@@ -3628,10 +3711,10 @@
       <c r="R17" s="3">
         <v>75</v>
       </c>
-      <c r="S17" s="33">
+      <c r="S17" s="32">
         <v>94</v>
       </c>
-      <c r="T17" s="32">
+      <c r="T17" s="31">
         <v>93</v>
       </c>
       <c r="U17" s="3">
@@ -3676,10 +3759,10 @@
       <c r="AH17" s="3">
         <v>90</v>
       </c>
-      <c r="AI17" s="33">
+      <c r="AI17" s="32">
         <v>90</v>
       </c>
-      <c r="AJ17" s="32">
+      <c r="AJ17" s="31">
         <v>100</v>
       </c>
       <c r="AK17" s="3">
@@ -3706,10 +3789,10 @@
       <c r="AR17" s="3">
         <v>86</v>
       </c>
-      <c r="AS17" s="22">
+      <c r="AS17" s="21">
         <v>99</v>
       </c>
-      <c r="AT17" s="32">
+      <c r="AT17" s="31">
         <v>92</v>
       </c>
       <c r="AU17" s="3">
@@ -3718,7 +3801,7 @@
       <c r="AV17" s="3">
         <v>55</v>
       </c>
-      <c r="AW17" s="22">
+      <c r="AW17" s="21">
         <v>55</v>
       </c>
       <c r="AX17" s="3">
@@ -3736,16 +3819,16 @@
       <c r="BB17" s="3">
         <v>98</v>
       </c>
-      <c r="BC17" s="33">
+      <c r="BC17" s="32">
         <v>98</v>
       </c>
     </row>
     <row r="18" spans="2:55" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="F18" s="57"/>
-      <c r="G18" s="31" t="s">
+      <c r="F18" s="70"/>
+      <c r="G18" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="38">
+      <c r="H18" s="37">
         <v>74</v>
       </c>
       <c r="I18" s="5">
@@ -3778,10 +3861,10 @@
       <c r="R18" s="5">
         <v>87</v>
       </c>
-      <c r="S18" s="39">
+      <c r="S18" s="38">
         <v>80</v>
       </c>
-      <c r="T18" s="38">
+      <c r="T18" s="37">
         <v>80</v>
       </c>
       <c r="U18" s="5">
@@ -3826,10 +3909,10 @@
       <c r="AH18" s="5">
         <v>88</v>
       </c>
-      <c r="AI18" s="39">
+      <c r="AI18" s="38">
         <v>88</v>
       </c>
-      <c r="AJ18" s="38">
+      <c r="AJ18" s="37">
         <v>68</v>
       </c>
       <c r="AK18" s="5">
@@ -3856,10 +3939,10 @@
       <c r="AR18" s="5">
         <v>80</v>
       </c>
-      <c r="AS18" s="23">
+      <c r="AS18" s="22">
         <v>72</v>
       </c>
-      <c r="AT18" s="38">
+      <c r="AT18" s="37">
         <v>68</v>
       </c>
       <c r="AU18" s="5">
@@ -3868,7 +3951,7 @@
       <c r="AV18" s="5">
         <v>67</v>
       </c>
-      <c r="AW18" s="23">
+      <c r="AW18" s="22">
         <v>67</v>
       </c>
       <c r="AX18" s="5">
@@ -3886,7 +3969,7 @@
       <c r="BB18" s="5">
         <v>76</v>
       </c>
-      <c r="BC18" s="39">
+      <c r="BC18" s="38">
         <v>75</v>
       </c>
     </row>
@@ -3952,54 +4035,61 @@
     </row>
     <row r="27" spans="2:55" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="2:55" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="2:55" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="2:55" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
-        <v>93</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="F30" s="7"/>
     </row>
     <row r="31" spans="2:55" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
-        <v>96</v>
-      </c>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="2:55" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="33" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B33" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="2:55" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="34" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B34" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="17"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B34" s="12" t="s">
+      <c r="C34" s="17"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B35" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="13"/>
-    </row>
-    <row r="35" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B35" s="14" t="s">
+      <c r="C35" s="13"/>
+    </row>
+    <row r="36" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B36" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="15"/>
+      <c r="C36" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="AT4:BC5"/>
     <mergeCell ref="F16:F18"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="F4:G4"/>
@@ -4013,7 +4103,6 @@
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="F15:G15"/>
-    <mergeCell ref="AT4:BC5"/>
   </mergeCells>
   <conditionalFormatting sqref="H16:BC16">
     <cfRule type="colorScale" priority="3">

</xml_diff>